<commit_message>
more mapping of pizzas
Updated the Knowledge Graph
</commit_message>
<xml_diff>
--- a/tabularDataToKG/pizzaMapping.xlsx
+++ b/tabularDataToKG/pizzaMapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\link4\Documents\CodeStuff\SWTKG\Pizza_KG\tabularDataToKG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\Pizza_KG\tabularDataToKG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88294944-1FD5-43ED-9A52-42065F0E7767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC10888-3452-4332-B7CD-66C1A085B101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{0E19E3C9-6306-41B9-8F30-BE52D1977342}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="246">
   <si>
     <t>org</t>
   </si>
@@ -156,9 +156,6 @@
     <t>auberginePizza</t>
   </si>
   <si>
-    <t>Eggplant Pizza</t>
-  </si>
-  <si>
     <t>Aubergine Pizza</t>
   </si>
   <si>
@@ -562,6 +559,210 @@
   </si>
   <si>
     <t>Kids</t>
+  </si>
+  <si>
+    <t>Taco Grande Pizza</t>
+  </si>
+  <si>
+    <t>glutenFreePizza</t>
+  </si>
+  <si>
+    <t>Gluten Free</t>
+  </si>
+  <si>
+    <t>cowboyPizza</t>
+  </si>
+  <si>
+    <t>Cowboy Pizza</t>
+  </si>
+  <si>
+    <t>pizzaiola</t>
+  </si>
+  <si>
+    <t>Pizzaiola</t>
+  </si>
+  <si>
+    <t>Pizza of the Week</t>
+  </si>
+  <si>
+    <t>Nutella Pizza</t>
+  </si>
+  <si>
+    <t>Pizza Italiano</t>
+  </si>
+  <si>
+    <t>Vegan Pizza</t>
+  </si>
+  <si>
+    <t>New York Style Pizza with</t>
+  </si>
+  <si>
+    <t>fiorentina</t>
+  </si>
+  <si>
+    <t>Stuffed Spinach Pizza</t>
+  </si>
+  <si>
+    <t>S39mores Pizza</t>
+  </si>
+  <si>
+    <t>viennese</t>
+  </si>
+  <si>
+    <t>Lasagna Pizza</t>
+  </si>
+  <si>
+    <t>Glutenfree Pizza</t>
+  </si>
+  <si>
+    <t>Pizza Capri</t>
+  </si>
+  <si>
+    <t>Dough Sticks</t>
+  </si>
+  <si>
+    <t>doughSticks</t>
+  </si>
+  <si>
+    <t>Basset Hound Pizza</t>
+  </si>
+  <si>
+    <t>bakedPotatoPizza</t>
+  </si>
+  <si>
+    <t>Baked Potato Pizza</t>
+  </si>
+  <si>
+    <t>Bad Boy Pizza</t>
+  </si>
+  <si>
+    <t>bruschettaPizza</t>
+  </si>
+  <si>
+    <t>Bruschetta</t>
+  </si>
+  <si>
+    <t>bbqPizza</t>
+  </si>
+  <si>
+    <t>BBQ Pizza</t>
+  </si>
+  <si>
+    <t>Mediterranean</t>
+  </si>
+  <si>
+    <t>Pizza Bread Sticks</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Pizza Pie</t>
+  </si>
+  <si>
+    <t>Pizza a La Totos</t>
+  </si>
+  <si>
+    <t>Thin Crust Pizza</t>
+  </si>
+  <si>
+    <t>Primavera</t>
+  </si>
+  <si>
+    <t>American Pizza</t>
+  </si>
+  <si>
+    <t>White Stone Pizza</t>
+  </si>
+  <si>
+    <t>Dessert Pizza</t>
+  </si>
+  <si>
+    <t>Barbeque Pizza</t>
+  </si>
+  <si>
+    <t>Favorite 4 Pizza</t>
+  </si>
+  <si>
+    <t>Florentine</t>
+  </si>
+  <si>
+    <t>Item Pizza</t>
+  </si>
+  <si>
+    <t>Snack Pizza</t>
+  </si>
+  <si>
+    <t>bbq</t>
+  </si>
+  <si>
+    <t>Meatza Pizza</t>
+  </si>
+  <si>
+    <t>Pizza Al Pesto</t>
+  </si>
+  <si>
+    <t>N. Y.</t>
+  </si>
+  <si>
+    <t>Eggplant</t>
+  </si>
+  <si>
+    <t>Spicy Sausage Pizza</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>Aloha Pizza</t>
+  </si>
+  <si>
+    <t>meat lover</t>
+  </si>
+  <si>
+    <t>vegetarian</t>
+  </si>
+  <si>
+    <t>Stuff Your Own Pizza</t>
+  </si>
+  <si>
+    <t>Chocolate Pizza</t>
+  </si>
+  <si>
+    <t>Pepperoni</t>
+  </si>
+  <si>
+    <t>Margharita</t>
+  </si>
+  <si>
+    <t>Hawaiian</t>
+  </si>
+  <si>
+    <t>pizzaSteak</t>
+  </si>
+  <si>
+    <t>steak</t>
+  </si>
+  <si>
+    <t>meat feast</t>
+  </si>
+  <si>
+    <t>ranch</t>
+  </si>
+  <si>
+    <t>alfredo</t>
+  </si>
+  <si>
+    <t>ameri</t>
+  </si>
+  <si>
+    <t>breakfastPizza</t>
+  </si>
+  <si>
+    <t>breakfast</t>
+  </si>
+  <si>
+    <t>Hawai</t>
   </si>
 </sst>
 </file>
@@ -913,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4723EA87-31D1-4211-9541-F76BF6230AB7}">
-  <dimension ref="A1:B143"/>
+  <dimension ref="A1:B200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="B143" sqref="B143"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,7 +1343,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>226</v>
       </c>
       <c r="B28" t="s">
         <v>42</v>
@@ -1150,7 +1351,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
         <v>42</v>
@@ -1158,15 +1359,15 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
@@ -1174,15 +1375,15 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
         <v>40</v>
@@ -1190,7 +1391,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
         <v>21</v>
@@ -1198,31 +1399,31 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" t="s">
         <v>55</v>
-      </c>
-      <c r="B37" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
         <v>21</v>
@@ -1230,7 +1431,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
         <v>21</v>
@@ -1238,7 +1439,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
         <v>17</v>
@@ -1246,31 +1447,31 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" t="s">
         <v>61</v>
-      </c>
-      <c r="B42" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B44" t="s">
         <v>37</v>
@@ -1278,71 +1479,71 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" t="s">
         <v>68</v>
-      </c>
-      <c r="B46" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" t="s">
         <v>76</v>
-      </c>
-      <c r="B52" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B53" t="s">
         <v>31</v>
@@ -1350,7 +1551,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B54" t="s">
         <v>21</v>
@@ -1358,7 +1559,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B55" t="s">
         <v>21</v>
@@ -1366,7 +1567,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B56" t="s">
         <v>21</v>
@@ -1374,55 +1575,55 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" t="s">
         <v>88</v>
-      </c>
-      <c r="B60" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B62" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B63" t="s">
         <v>21</v>
@@ -1430,31 +1631,31 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B67" t="s">
         <v>21</v>
@@ -1462,7 +1663,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B68" t="s">
         <v>21</v>
@@ -1470,7 +1671,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B69" t="s">
         <v>21</v>
@@ -1478,7 +1679,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B70" t="s">
         <v>21</v>
@@ -1486,23 +1687,23 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B73" t="s">
         <v>21</v>
@@ -1510,31 +1711,31 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B74" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>105</v>
+      </c>
+      <c r="B75" t="s">
         <v>106</v>
-      </c>
-      <c r="B75" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B76" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B77" t="s">
         <v>37</v>
@@ -1542,7 +1743,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B78" t="s">
         <v>4</v>
@@ -1550,7 +1751,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B79" t="s">
         <v>31</v>
@@ -1558,7 +1759,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B80" t="s">
         <v>34</v>
@@ -1566,39 +1767,39 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B81" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>114</v>
+      </c>
+      <c r="B82" t="s">
         <v>115</v>
-      </c>
-      <c r="B82" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B83" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B84" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B85" t="s">
         <v>21</v>
@@ -1606,15 +1807,15 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B86" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B87" t="s">
         <v>21</v>
@@ -1622,23 +1823,23 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B88" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B89" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B90" t="s">
         <v>21</v>
@@ -1646,7 +1847,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B91" t="s">
         <v>21</v>
@@ -1654,23 +1855,23 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B92" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B93" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B94" t="s">
         <v>21</v>
@@ -1678,39 +1879,39 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B95" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B96" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B97" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B98" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B99" t="s">
         <v>10</v>
@@ -1718,15 +1919,15 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B100" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B101" t="s">
         <v>21</v>
@@ -1734,31 +1935,31 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B102" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B103" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B104" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B105" t="s">
         <v>6</v>
@@ -1766,23 +1967,23 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B106" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B107" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B108" t="s">
         <v>21</v>
@@ -1790,7 +1991,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B109" t="s">
         <v>40</v>
@@ -1798,15 +1999,15 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B110" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B111" t="s">
         <v>10</v>
@@ -1814,31 +2015,31 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B112" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B113" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B114" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B115" t="s">
         <v>21</v>
@@ -1846,7 +2047,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B116" t="s">
         <v>17</v>
@@ -1854,10 +2055,10 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -1870,7 +2071,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B119" t="s">
         <v>10</v>
@@ -1878,7 +2079,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
@@ -1886,26 +2087,26 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B121" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B122" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B123" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -1918,31 +2119,31 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B125" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B126" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B127" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B128" t="s">
         <v>21</v>
@@ -1950,7 +2151,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B129" t="s">
         <v>4</v>
@@ -1958,7 +2159,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B130" t="s">
         <v>6</v>
@@ -1966,7 +2167,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B131" t="s">
         <v>6</v>
@@ -1974,15 +2175,15 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B132" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B133" t="s">
         <v>21</v>
@@ -1990,15 +2191,15 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B134" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B135" t="s">
         <v>10</v>
@@ -2006,31 +2207,31 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B136" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B137" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B138" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B139" t="s">
         <v>21</v>
@@ -2038,7 +2239,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B140" t="s">
         <v>4</v>
@@ -2046,7 +2247,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B141" t="s">
         <v>21</v>
@@ -2054,18 +2255,474 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>175</v>
+      </c>
+      <c r="B142" t="s">
         <v>176</v>
-      </c>
-      <c r="B142" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B143" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>178</v>
+      </c>
+      <c r="B144" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>180</v>
+      </c>
+      <c r="B145" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>182</v>
+      </c>
+      <c r="B146" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>184</v>
+      </c>
+      <c r="B147" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>185</v>
+      </c>
+      <c r="B148" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>186</v>
+      </c>
+      <c r="B149" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>187</v>
+      </c>
+      <c r="B150" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>188</v>
+      </c>
+      <c r="B151" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>189</v>
+      </c>
+      <c r="B152" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>190</v>
+      </c>
+      <c r="B153" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>191</v>
+      </c>
+      <c r="B154" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>192</v>
+      </c>
+      <c r="B155" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>194</v>
+      </c>
+      <c r="B156" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>209</v>
+      </c>
+      <c r="B157" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>195</v>
+      </c>
+      <c r="B158" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>196</v>
+      </c>
+      <c r="B159" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>197</v>
+      </c>
+      <c r="B160" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>199</v>
+      </c>
+      <c r="B161" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>201</v>
+      </c>
+      <c r="B162" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>202</v>
+      </c>
+      <c r="B163" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>204</v>
+      </c>
+      <c r="B164" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>206</v>
+      </c>
+      <c r="B165" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>207</v>
+      </c>
+      <c r="B166" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>208</v>
+      </c>
+      <c r="B167" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>210</v>
+      </c>
+      <c r="B168" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>211</v>
+      </c>
+      <c r="B169" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>212</v>
+      </c>
+      <c r="B170" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>213</v>
+      </c>
+      <c r="B171" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>214</v>
+      </c>
+      <c r="B172" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>215</v>
+      </c>
+      <c r="B173" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>216</v>
+      </c>
+      <c r="B174" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>217</v>
+      </c>
+      <c r="B175" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>218</v>
+      </c>
+      <c r="B176" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>219</v>
+      </c>
+      <c r="B177" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>220</v>
+      </c>
+      <c r="B178" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>221</v>
+      </c>
+      <c r="B179" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>222</v>
+      </c>
+      <c r="B180" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>223</v>
+      </c>
+      <c r="B181" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>224</v>
+      </c>
+      <c r="B182" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>225</v>
+      </c>
+      <c r="B183" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>227</v>
+      </c>
+      <c r="B184" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>228</v>
+      </c>
+      <c r="B185" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>229</v>
+      </c>
+      <c r="B186" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>230</v>
+      </c>
+      <c r="B187" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>231</v>
+      </c>
+      <c r="B188" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>232</v>
+      </c>
+      <c r="B189" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>233</v>
+      </c>
+      <c r="B190" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>234</v>
+      </c>
+      <c r="B191" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>235</v>
+      </c>
+      <c r="B192" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>236</v>
+      </c>
+      <c r="B193" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>238</v>
+      </c>
+      <c r="B194" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>239</v>
+      </c>
+      <c r="B195" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>240</v>
+      </c>
+      <c r="B196" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>241</v>
+      </c>
+      <c r="B197" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>242</v>
+      </c>
+      <c r="B198" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>244</v>
+      </c>
+      <c r="B199" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>245</v>
+      </c>
+      <c r="B200" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inserting menu items to knowledge graph
</commit_message>
<xml_diff>
--- a/tabularDataToKG/pizzaMapping.xlsx
+++ b/tabularDataToKG/pizzaMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\Pizza_KG\tabularDataToKG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC10888-3452-4332-B7CD-66C1A085B101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA1CC5E-5D03-47A4-8D3D-C9A74663DCFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{0E19E3C9-6306-41B9-8F30-BE52D1977342}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="247">
   <si>
     <t>org</t>
   </si>
@@ -763,6 +763,9 @@
   </si>
   <si>
     <t>Hawai</t>
+  </si>
+  <si>
+    <t>chocolate</t>
   </si>
 </sst>
 </file>
@@ -1114,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4723EA87-31D1-4211-9541-F76BF6230AB7}">
-  <dimension ref="A1:B200"/>
+  <dimension ref="A1:B201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="B201" sqref="B201"/>
+      <selection activeCell="A202" sqref="A202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2725,6 +2728,14 @@
         <v>31</v>
       </c>
     </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>246</v>
+      </c>
+      <c r="B201" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added in the ingredients to the mapping
</commit_message>
<xml_diff>
--- a/tabularDataToKG/pizzaMapping.xlsx
+++ b/tabularDataToKG/pizzaMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\Pizza_KG\tabularDataToKG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA1CC5E-5D03-47A4-8D3D-C9A74663DCFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D71D3D-9874-4BF5-9CE6-B1287FF90955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{0E19E3C9-6306-41B9-8F30-BE52D1977342}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{0E19E3C9-6306-41B9-8F30-BE52D1977342}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="278">
   <si>
     <t>org</t>
   </si>
@@ -766,6 +766,99 @@
   </si>
   <si>
     <t>chocolate</t>
+  </si>
+  <si>
+    <t>american hot</t>
+  </si>
+  <si>
+    <t>americanHot</t>
+  </si>
+  <si>
+    <t>cajun</t>
+  </si>
+  <si>
+    <t>caprina</t>
+  </si>
+  <si>
+    <t>curry</t>
+  </si>
+  <si>
+    <t>fishi</t>
+  </si>
+  <si>
+    <t>eFichi</t>
+  </si>
+  <si>
+    <t>giardiniera</t>
+  </si>
+  <si>
+    <t>reine</t>
+  </si>
+  <si>
+    <t>laReine</t>
+  </si>
+  <si>
+    <t>napoletana</t>
+  </si>
+  <si>
+    <t>parmese</t>
+  </si>
+  <si>
+    <t>ham</t>
+  </si>
+  <si>
+    <t>pisan</t>
+  </si>
+  <si>
+    <t>pugliese</t>
+  </si>
+  <si>
+    <t>onion</t>
+  </si>
+  <si>
+    <t>roma</t>
+  </si>
+  <si>
+    <t>romana</t>
+  </si>
+  <si>
+    <t>carlo</t>
+  </si>
+  <si>
+    <t>princeCarlo</t>
+  </si>
+  <si>
+    <t>leek</t>
+  </si>
+  <si>
+    <t>rosa</t>
+  </si>
+  <si>
+    <t>gorgonzola</t>
+  </si>
+  <si>
+    <t>sloppy</t>
+  </si>
+  <si>
+    <t>sloppyGiuseppe</t>
+  </si>
+  <si>
+    <t>giuseppe</t>
+  </si>
+  <si>
+    <t>soho</t>
+  </si>
+  <si>
+    <t>rocket</t>
+  </si>
+  <si>
+    <t>venez</t>
+  </si>
+  <si>
+    <t>veneziana</t>
+  </si>
+  <si>
+    <t>caper</t>
   </si>
 </sst>
 </file>
@@ -1117,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4723EA87-31D1-4211-9541-F76BF6230AB7}">
-  <dimension ref="A1:B201"/>
+  <dimension ref="A1:B225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="A202" sqref="A202"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="A226" sqref="A226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2706,34 +2799,226 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B198" t="s">
-        <v>17</v>
+        <v>248</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B199" t="s">
-        <v>243</v>
+        <v>17</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B200" t="s">
-        <v>31</v>
+        <v>243</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
+        <v>245</v>
+      </c>
+      <c r="B201" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>246</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B202" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>249</v>
+      </c>
+      <c r="B203" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>250</v>
+      </c>
+      <c r="B204" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>251</v>
+      </c>
+      <c r="B205" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>252</v>
+      </c>
+      <c r="B206" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>254</v>
+      </c>
+      <c r="B207" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>255</v>
+      </c>
+      <c r="B208" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>257</v>
+      </c>
+      <c r="B209" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>258</v>
+      </c>
+      <c r="B210" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>259</v>
+      </c>
+      <c r="B211" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>260</v>
+      </c>
+      <c r="B212" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>261</v>
+      </c>
+      <c r="B213" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>262</v>
+      </c>
+      <c r="B214" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>263</v>
+      </c>
+      <c r="B215" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>265</v>
+      </c>
+      <c r="B216" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>267</v>
+      </c>
+      <c r="B217" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>268</v>
+      </c>
+      <c r="B218" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>269</v>
+      </c>
+      <c r="B219" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>270</v>
+      </c>
+      <c r="B220" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>272</v>
+      </c>
+      <c r="B221" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>273</v>
+      </c>
+      <c r="B222" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>274</v>
+      </c>
+      <c r="B223" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>275</v>
+      </c>
+      <c r="B224" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>277</v>
+      </c>
+      <c r="B225" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sorted out some issues with tabular data to kg
Started inference
</commit_message>
<xml_diff>
--- a/tabularDataToKG/pizzaMapping.xlsx
+++ b/tabularDataToKG/pizzaMapping.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\Pizza_KG\tabularDataToKG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D71D3D-9874-4BF5-9CE6-B1287FF90955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB3356C-0038-4890-862C-EFEFB8F475C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{0E19E3C9-6306-41B9-8F30-BE52D1977342}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0E19E3C9-6306-41B9-8F30-BE52D1977342}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$225</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="277">
   <si>
     <t>org</t>
   </si>
@@ -142,9 +145,6 @@
   </si>
   <si>
     <t>Create Your Own Pizza</t>
-  </si>
-  <si>
-    <t>Pizza</t>
   </si>
   <si>
     <t>buffaloChickenPizza</t>
@@ -1212,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4723EA87-31D1-4211-9541-F76BF6230AB7}">
   <dimension ref="A1:B225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="A226" sqref="A226"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,7 +1370,7 @@
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1426,44 +1426,44 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
@@ -1471,23 +1471,23 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
         <v>21</v>
@@ -1495,31 +1495,31 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
         <v>54</v>
-      </c>
-      <c r="B37" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
         <v>21</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
         <v>21</v>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
         <v>17</v>
@@ -1543,31 +1543,31 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" t="s">
         <v>60</v>
-      </c>
-      <c r="B42" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
         <v>37</v>
@@ -1575,71 +1575,71 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" t="s">
         <v>67</v>
-      </c>
-      <c r="B46" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" t="s">
         <v>75</v>
-      </c>
-      <c r="B52" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B53" t="s">
         <v>31</v>
@@ -1647,7 +1647,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B54" t="s">
         <v>21</v>
@@ -1655,7 +1655,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B55" t="s">
         <v>21</v>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B56" t="s">
         <v>21</v>
@@ -1671,55 +1671,55 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B57" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>86</v>
+      </c>
+      <c r="B60" t="s">
         <v>87</v>
-      </c>
-      <c r="B60" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B63" t="s">
         <v>21</v>
@@ -1727,31 +1727,31 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B67" t="s">
         <v>21</v>
@@ -1759,7 +1759,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B68" t="s">
         <v>21</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B69" t="s">
         <v>21</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B70" t="s">
         <v>21</v>
@@ -1783,23 +1783,23 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B71" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B72" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B73" t="s">
         <v>21</v>
@@ -1807,31 +1807,31 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B74" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>104</v>
+      </c>
+      <c r="B75" t="s">
         <v>105</v>
-      </c>
-      <c r="B75" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B76" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B77" t="s">
         <v>37</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B78" t="s">
         <v>4</v>
@@ -1847,7 +1847,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B79" t="s">
         <v>31</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B80" t="s">
         <v>34</v>
@@ -1863,39 +1863,39 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B81" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>113</v>
+      </c>
+      <c r="B82" t="s">
         <v>114</v>
-      </c>
-      <c r="B82" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B83" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B84" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B85" t="s">
         <v>21</v>
@@ -1903,15 +1903,15 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B86" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B87" t="s">
         <v>21</v>
@@ -1919,23 +1919,23 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B88" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B89" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B90" t="s">
         <v>21</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B91" t="s">
         <v>21</v>
@@ -1951,23 +1951,23 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B92" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B93" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B94" t="s">
         <v>21</v>
@@ -1975,39 +1975,39 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B95" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B96" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B97" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B98" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B99" t="s">
         <v>10</v>
@@ -2015,15 +2015,15 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B101" t="s">
         <v>21</v>
@@ -2031,31 +2031,31 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B102" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B103" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B104" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B105" t="s">
         <v>6</v>
@@ -2063,23 +2063,23 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B106" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B107" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B108" t="s">
         <v>21</v>
@@ -2087,23 +2087,23 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B109" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B110" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B111" t="s">
         <v>10</v>
@@ -2111,31 +2111,31 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B112" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B113" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B114" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B115" t="s">
         <v>21</v>
@@ -2143,7 +2143,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B116" t="s">
         <v>17</v>
@@ -2151,10 +2151,10 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B117" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -2167,7 +2167,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B119" t="s">
         <v>10</v>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
@@ -2183,26 +2183,26 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B121" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B122" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B123" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2215,31 +2215,31 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B125" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B126" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B127" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B128" t="s">
         <v>21</v>
@@ -2247,7 +2247,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B129" t="s">
         <v>4</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B130" t="s">
         <v>6</v>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B131" t="s">
         <v>6</v>
@@ -2271,15 +2271,15 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B132" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B133" t="s">
         <v>21</v>
@@ -2287,15 +2287,15 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B134" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B135" t="s">
         <v>10</v>
@@ -2303,31 +2303,31 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B136" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B137" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B138" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B139" t="s">
         <v>21</v>
@@ -2335,7 +2335,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B140" t="s">
         <v>4</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B141" t="s">
         <v>21</v>
@@ -2351,15 +2351,15 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>174</v>
+      </c>
+      <c r="B142" t="s">
         <v>175</v>
-      </c>
-      <c r="B142" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B143" t="s">
         <v>10</v>
@@ -2367,39 +2367,39 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B144" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B145" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B146" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B147" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B148" t="s">
         <v>21</v>
@@ -2407,7 +2407,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B149" t="s">
         <v>37</v>
@@ -2415,7 +2415,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B150" t="s">
         <v>21</v>
@@ -2423,15 +2423,15 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B151" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B152" t="s">
         <v>21</v>
@@ -2439,23 +2439,23 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B153" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B154" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B155" t="s">
         <v>21</v>
@@ -2463,15 +2463,15 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B156" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B157" t="s">
         <v>21</v>
@@ -2479,15 +2479,15 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B158" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B159" t="s">
         <v>10</v>
@@ -2495,15 +2495,15 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>196</v>
+      </c>
+      <c r="B160" t="s">
         <v>197</v>
-      </c>
-      <c r="B160" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B161" t="s">
         <v>21</v>
@@ -2511,15 +2511,15 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B162" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B163" t="s">
         <v>21</v>
@@ -2527,39 +2527,39 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B164" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B165" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B166" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B167" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B168" t="s">
         <v>21</v>
@@ -2567,7 +2567,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B169" t="s">
         <v>21</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B170" t="s">
         <v>21</v>
@@ -2583,7 +2583,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B171" t="s">
         <v>14</v>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B172" t="s">
         <v>17</v>
@@ -2599,7 +2599,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B173" t="s">
         <v>6</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B174" t="s">
         <v>37</v>
@@ -2615,31 +2615,31 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B175" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B176" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B177" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B178" t="s">
         <v>21</v>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B179" t="s">
         <v>10</v>
@@ -2655,31 +2655,31 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B180" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B181" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B182" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B183" t="s">
         <v>21</v>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B184" t="s">
         <v>17</v>
@@ -2695,15 +2695,15 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B185" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B186" t="s">
         <v>31</v>
@@ -2711,23 +2711,23 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B187" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B188" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B189" t="s">
         <v>21</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B190" t="s">
         <v>37</v>
@@ -2743,7 +2743,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B191" t="s">
         <v>17</v>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B192" t="s">
         <v>4</v>
@@ -2759,7 +2759,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B193" t="s">
         <v>31</v>
@@ -2767,47 +2767,47 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B194" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B195" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B196" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B197" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
+        <v>246</v>
+      </c>
+      <c r="B198" t="s">
         <v>247</v>
-      </c>
-      <c r="B198" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B199" t="s">
         <v>17</v>
@@ -2815,15 +2815,15 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B200" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B201" t="s">
         <v>31</v>
@@ -2831,7 +2831,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B202" t="s">
         <v>37</v>
@@ -2839,189 +2839,190 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B203" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B204" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B205" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
+        <v>251</v>
+      </c>
+      <c r="B206" t="s">
         <v>252</v>
-      </c>
-      <c r="B206" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B207" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>254</v>
+      </c>
+      <c r="B208" t="s">
         <v>255</v>
-      </c>
-      <c r="B208" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B209" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B210" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B211" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B212" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B213" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B214" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
+        <v>262</v>
+      </c>
+      <c r="B215" t="s">
         <v>263</v>
-      </c>
-      <c r="B215" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
+        <v>264</v>
+      </c>
+      <c r="B216" t="s">
         <v>265</v>
-      </c>
-      <c r="B216" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B217" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B218" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B219" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
+        <v>269</v>
+      </c>
+      <c r="B220" t="s">
         <v>270</v>
-      </c>
-      <c r="B220" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B221" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B222" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B223" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
+        <v>274</v>
+      </c>
+      <c r="B224" t="s">
         <v>275</v>
-      </c>
-      <c r="B224" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B225" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B225" xr:uid="{4723EA87-31D1-4211-9541-F76BF6230AB7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>